<commit_message>
comparing my predictions to actual ncv values
</commit_message>
<xml_diff>
--- a/allcontrols.xlsx
+++ b/allcontrols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83CB3F5-AB03-47FE-BF43-694EAFAECA3C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23694B1-A42D-4350-875B-E5FB7335F4E1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11292" windowHeight="9492" xr2:uid="{A274F495-8BA5-45B2-8E80-3B8BD1F44BC5}"/>
   </bookViews>
@@ -379,20 +379,20 @@
   <dimension ref="A2:BW132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:BW301"/>
+      <selection sqref="A1:C301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="2" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
-        <v>278</v>
+        <v>135</v>
       </c>
       <c r="B2">
-        <v>302</v>
+        <v>522</v>
       </c>
       <c r="C2">
-        <v>293</v>
+        <v>142</v>
       </c>
       <c r="D2">
         <v>137</v>
@@ -610,13 +610,13 @@
     </row>
     <row r="3" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
-        <v>284</v>
+        <v>138</v>
       </c>
       <c r="B3">
-        <v>115</v>
+        <v>518</v>
       </c>
       <c r="C3">
-        <v>294</v>
+        <v>144</v>
       </c>
       <c r="D3">
         <v>136</v>
@@ -834,13 +834,13 @@
     </row>
     <row r="4" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
-        <v>283</v>
+        <v>133</v>
       </c>
       <c r="B4">
-        <v>117</v>
+        <v>493</v>
       </c>
       <c r="C4">
-        <v>296</v>
+        <v>143</v>
       </c>
       <c r="D4">
         <v>136</v>
@@ -1058,13 +1058,13 @@
     </row>
     <row r="5" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
-        <v>248</v>
+        <v>136</v>
       </c>
       <c r="B5">
-        <v>117</v>
+        <v>333</v>
       </c>
       <c r="C5">
-        <v>295</v>
+        <v>143</v>
       </c>
       <c r="D5">
         <v>137</v>
@@ -1279,13 +1279,13 @@
     </row>
     <row r="6" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
-        <v>181</v>
+        <v>139</v>
       </c>
       <c r="B6">
-        <v>115</v>
+        <v>375</v>
       </c>
       <c r="C6">
-        <v>299</v>
+        <v>89</v>
       </c>
       <c r="D6">
         <v>137</v>
@@ -1497,13 +1497,13 @@
     </row>
     <row r="7" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
-        <v>248</v>
+        <v>110</v>
       </c>
       <c r="B7">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C7">
-        <v>298</v>
+        <v>143</v>
       </c>
       <c r="D7">
         <v>137</v>
@@ -1712,13 +1712,13 @@
     </row>
     <row r="8" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
-        <v>248</v>
+        <v>109</v>
       </c>
       <c r="B8">
-        <v>115</v>
+        <v>332</v>
       </c>
       <c r="C8">
-        <v>302</v>
+        <v>141</v>
       </c>
       <c r="D8">
         <v>136</v>
@@ -1927,13 +1927,13 @@
     </row>
     <row r="9" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
-        <v>248</v>
+        <v>140</v>
       </c>
       <c r="B9">
-        <v>117</v>
+        <v>333</v>
       </c>
       <c r="C9">
-        <v>303</v>
+        <v>141</v>
       </c>
       <c r="D9">
         <v>137</v>
@@ -2139,13 +2139,13 @@
     </row>
     <row r="10" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
-        <v>248</v>
+        <v>141</v>
       </c>
       <c r="B10">
-        <v>304</v>
+        <v>336</v>
       </c>
       <c r="C10">
-        <v>305</v>
+        <v>141</v>
       </c>
       <c r="D10">
         <v>137</v>
@@ -2351,13 +2351,13 @@
     </row>
     <row r="11" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
-        <v>249</v>
+        <v>77</v>
       </c>
       <c r="B11">
-        <v>117</v>
+        <v>333</v>
       </c>
       <c r="C11">
-        <v>307</v>
+        <v>141</v>
       </c>
       <c r="D11">
         <v>136</v>
@@ -2560,13 +2560,13 @@
     </row>
     <row r="12" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
-        <v>250</v>
+        <v>139</v>
       </c>
       <c r="B12">
-        <v>116</v>
+        <v>333</v>
       </c>
       <c r="C12">
-        <v>306</v>
+        <v>143</v>
       </c>
       <c r="D12">
         <v>136</v>
@@ -2769,13 +2769,13 @@
     </row>
     <row r="13" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
-        <v>252</v>
+        <v>110</v>
       </c>
       <c r="B13">
-        <v>115</v>
+        <v>241</v>
       </c>
       <c r="C13">
-        <v>309</v>
+        <v>617</v>
       </c>
       <c r="D13">
         <v>137</v>
@@ -2978,13 +2978,13 @@
     </row>
     <row r="14" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
-        <v>249</v>
+        <v>106</v>
       </c>
       <c r="B14">
-        <v>116</v>
+        <v>331</v>
       </c>
       <c r="C14">
-        <v>309</v>
+        <v>144</v>
       </c>
       <c r="D14">
         <v>137</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="15" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
-        <v>248</v>
+        <v>139</v>
       </c>
       <c r="B15">
-        <v>99</v>
+        <v>428</v>
       </c>
       <c r="C15">
-        <v>317</v>
+        <v>143</v>
       </c>
       <c r="D15">
         <v>136</v>
@@ -3390,13 +3390,13 @@
     </row>
     <row r="16" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
-        <v>248</v>
+        <v>78</v>
       </c>
       <c r="B16">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="C16">
-        <v>315</v>
+        <v>91</v>
       </c>
       <c r="D16">
         <v>137</v>
@@ -3596,13 +3596,13 @@
     </row>
     <row r="17" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
-        <v>246</v>
+        <v>109</v>
       </c>
       <c r="B17">
-        <v>115</v>
+        <v>269</v>
       </c>
       <c r="C17">
-        <v>320</v>
+        <v>141</v>
       </c>
       <c r="D17">
         <v>137</v>
@@ -3802,13 +3802,13 @@
     </row>
     <row r="18" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
-        <v>248</v>
+        <v>114</v>
       </c>
       <c r="B18">
-        <v>115</v>
+        <v>271</v>
       </c>
       <c r="C18">
-        <v>320</v>
+        <v>88</v>
       </c>
       <c r="D18">
         <v>137</v>
@@ -4008,13 +4008,13 @@
     </row>
     <row r="19" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
-        <v>250</v>
+        <v>109</v>
       </c>
       <c r="B19">
-        <v>120</v>
+        <v>270</v>
       </c>
       <c r="C19">
-        <v>325</v>
+        <v>143</v>
       </c>
       <c r="D19">
         <v>136</v>
@@ -4208,13 +4208,13 @@
     </row>
     <row r="20" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
-        <v>251</v>
+        <v>118</v>
       </c>
       <c r="B20">
-        <v>114</v>
+        <v>242</v>
       </c>
       <c r="C20">
-        <v>324</v>
+        <v>139</v>
       </c>
       <c r="D20">
         <v>137</v>
@@ -4408,13 +4408,13 @@
     </row>
     <row r="21" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
-        <v>247</v>
+        <v>140</v>
       </c>
       <c r="B21">
-        <v>114</v>
+        <v>337</v>
       </c>
       <c r="C21">
-        <v>328</v>
+        <v>614</v>
       </c>
       <c r="D21">
         <v>137</v>
@@ -4608,13 +4608,13 @@
     </row>
     <row r="22" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="B22">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="C22">
-        <v>333</v>
+        <v>144</v>
       </c>
       <c r="D22">
         <v>137</v>
@@ -4808,13 +4808,13 @@
     </row>
     <row r="23" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
-        <v>250</v>
+        <v>113</v>
       </c>
       <c r="B23">
-        <v>114</v>
+        <v>333</v>
       </c>
       <c r="C23">
-        <v>336</v>
+        <v>232</v>
       </c>
       <c r="D23">
         <v>136</v>
@@ -5008,13 +5008,13 @@
     </row>
     <row r="24" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
-        <v>250</v>
+        <v>110</v>
       </c>
       <c r="B24">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="C24">
-        <v>335</v>
+        <v>142</v>
       </c>
       <c r="D24">
         <v>137</v>
@@ -5208,13 +5208,13 @@
     </row>
     <row r="25" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
-        <v>249</v>
+        <v>110</v>
       </c>
       <c r="B25">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="C25">
-        <v>337</v>
+        <v>144</v>
       </c>
       <c r="D25">
         <v>137</v>
@@ -5408,13 +5408,13 @@
     </row>
     <row r="26" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
-        <v>249</v>
+        <v>110</v>
       </c>
       <c r="B26">
-        <v>113</v>
+        <v>335</v>
       </c>
       <c r="C26">
-        <v>323</v>
+        <v>84</v>
       </c>
       <c r="D26">
         <v>137</v>
@@ -5602,13 +5602,13 @@
     </row>
     <row r="27" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
-        <v>251</v>
+        <v>110</v>
       </c>
       <c r="B27">
-        <v>114</v>
+        <v>337</v>
       </c>
       <c r="C27">
-        <v>340</v>
+        <v>95</v>
       </c>
       <c r="D27">
         <v>137</v>
@@ -5796,13 +5796,13 @@
     </row>
     <row r="28" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
-        <v>248</v>
+        <v>111</v>
       </c>
       <c r="B28">
-        <v>110</v>
+        <v>273</v>
       </c>
       <c r="C28">
-        <v>340</v>
+        <v>621</v>
       </c>
       <c r="D28">
         <v>137</v>
@@ -5987,13 +5987,13 @@
     </row>
     <row r="29" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
-        <v>248</v>
+        <v>114</v>
       </c>
       <c r="B29">
-        <v>114</v>
+        <v>336</v>
       </c>
       <c r="C29">
-        <v>347</v>
+        <v>141</v>
       </c>
       <c r="D29">
         <v>137</v>
@@ -6178,13 +6178,13 @@
     </row>
     <row r="30" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
-        <v>246</v>
+        <v>108</v>
       </c>
       <c r="B30">
-        <v>305</v>
+        <v>133</v>
       </c>
       <c r="C30">
-        <v>348</v>
+        <v>139</v>
       </c>
       <c r="D30">
         <v>137</v>
@@ -6369,13 +6369,13 @@
     </row>
     <row r="31" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
-        <v>251</v>
+        <v>142</v>
       </c>
       <c r="B31">
-        <v>113</v>
+        <v>337</v>
       </c>
       <c r="C31">
-        <v>349</v>
+        <v>88</v>
       </c>
       <c r="D31">
         <v>136</v>
@@ -6557,13 +6557,13 @@
     </row>
     <row r="32" spans="1:75" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
-        <v>250</v>
+        <v>108</v>
       </c>
       <c r="B32">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="C32">
-        <v>349</v>
+        <v>100</v>
       </c>
       <c r="D32">
         <v>137</v>
@@ -6745,13 +6745,13 @@
     </row>
     <row r="33" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
-        <v>250</v>
+        <v>111</v>
       </c>
       <c r="B33">
-        <v>306</v>
+        <v>132</v>
       </c>
       <c r="C33">
-        <v>354</v>
+        <v>93</v>
       </c>
       <c r="D33">
         <v>137</v>
@@ -6927,13 +6927,13 @@
     </row>
     <row r="34" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
-        <v>251</v>
+        <v>110</v>
       </c>
       <c r="B34">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="C34">
-        <v>353</v>
+        <v>140</v>
       </c>
       <c r="D34">
         <v>137</v>
@@ -7109,13 +7109,13 @@
     </row>
     <row r="35" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
-        <v>250</v>
+        <v>111</v>
       </c>
       <c r="B35">
-        <v>115</v>
+        <v>521</v>
       </c>
       <c r="C35">
-        <v>356</v>
+        <v>92</v>
       </c>
       <c r="D35">
         <v>137</v>
@@ -7288,13 +7288,13 @@
     </row>
     <row r="36" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
-        <v>249</v>
+        <v>111</v>
       </c>
       <c r="B36">
-        <v>304</v>
+        <v>276</v>
       </c>
       <c r="C36">
-        <v>350</v>
+        <v>141</v>
       </c>
       <c r="D36">
         <v>136</v>
@@ -7467,13 +7467,13 @@
     </row>
     <row r="37" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
-        <v>250</v>
+        <v>112</v>
       </c>
       <c r="B37">
-        <v>115</v>
+        <v>275</v>
       </c>
       <c r="C37">
-        <v>367</v>
+        <v>89</v>
       </c>
       <c r="D37">
         <v>136</v>
@@ -7646,13 +7646,13 @@
     </row>
     <row r="38" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
-        <v>251</v>
+        <v>113</v>
       </c>
       <c r="B38">
-        <v>113</v>
+        <v>276</v>
       </c>
       <c r="C38">
-        <v>356</v>
+        <v>87</v>
       </c>
       <c r="D38">
         <v>137</v>
@@ -7822,13 +7822,13 @@
     </row>
     <row r="39" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
-        <v>281</v>
+        <v>113</v>
       </c>
       <c r="B39">
-        <v>115</v>
+        <v>273</v>
       </c>
       <c r="C39">
-        <v>361</v>
+        <v>87</v>
       </c>
       <c r="D39">
         <v>137</v>
@@ -7998,13 +7998,13 @@
     </row>
     <row r="40" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
-        <v>250</v>
+        <v>139</v>
       </c>
       <c r="B40">
-        <v>116</v>
+        <v>278</v>
       </c>
       <c r="C40">
-        <v>362</v>
+        <v>82</v>
       </c>
       <c r="D40">
         <v>137</v>
@@ -8174,13 +8174,13 @@
     </row>
     <row r="41" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <v>251</v>
+        <v>111</v>
       </c>
       <c r="B41">
-        <v>112</v>
+        <v>277</v>
       </c>
       <c r="C41">
-        <v>360</v>
+        <v>141</v>
       </c>
       <c r="D41">
         <v>136</v>
@@ -8350,13 +8350,13 @@
     </row>
     <row r="42" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
-        <v>250</v>
+        <v>139</v>
       </c>
       <c r="B42">
-        <v>111</v>
+        <v>276</v>
       </c>
       <c r="C42">
-        <v>369</v>
+        <v>319</v>
       </c>
       <c r="D42">
         <v>137</v>
@@ -8526,13 +8526,13 @@
     </row>
     <row r="43" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
-        <v>249</v>
+        <v>114</v>
       </c>
       <c r="B43">
-        <v>102</v>
+        <v>337</v>
       </c>
       <c r="C43">
-        <v>377</v>
+        <v>81</v>
       </c>
       <c r="D43">
         <v>139</v>
@@ -8702,13 +8702,13 @@
     </row>
     <row r="44" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
-        <v>250</v>
+        <v>111</v>
       </c>
       <c r="B44">
-        <v>115</v>
+        <v>890</v>
       </c>
       <c r="C44">
-        <v>372</v>
+        <v>85</v>
       </c>
       <c r="D44">
         <v>137</v>
@@ -8878,13 +8878,13 @@
     </row>
     <row r="45" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
-        <v>249</v>
+        <v>119</v>
       </c>
       <c r="B45">
-        <v>114</v>
+        <v>846</v>
       </c>
       <c r="C45">
-        <v>367</v>
+        <v>138</v>
       </c>
       <c r="D45">
         <v>137</v>
@@ -9051,13 +9051,10 @@
     </row>
     <row r="46" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
-        <v>251</v>
-      </c>
-      <c r="B46">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="C46">
-        <v>372</v>
+        <v>140</v>
       </c>
       <c r="D46">
         <v>138</v>
@@ -9218,13 +9215,10 @@
     </row>
     <row r="47" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
-        <v>251</v>
-      </c>
-      <c r="B47">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="C47">
-        <v>360</v>
+        <v>89</v>
       </c>
       <c r="D47">
         <v>137</v>
@@ -9382,13 +9376,10 @@
     </row>
     <row r="48" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
-        <v>249</v>
-      </c>
-      <c r="B48">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="C48">
-        <v>373</v>
+        <v>86</v>
       </c>
       <c r="D48">
         <v>137</v>
@@ -9540,13 +9531,10 @@
     </row>
     <row r="49" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
-        <v>250</v>
-      </c>
-      <c r="B49">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="C49">
-        <v>375</v>
+        <v>137</v>
       </c>
       <c r="D49">
         <v>137</v>
@@ -9695,13 +9683,10 @@
     </row>
     <row r="50" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
-        <v>250</v>
-      </c>
-      <c r="B50">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="C50">
-        <v>378</v>
+        <v>137</v>
       </c>
       <c r="D50">
         <v>137</v>
@@ -9844,13 +9829,10 @@
     </row>
     <row r="51" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
-        <v>251</v>
-      </c>
-      <c r="B51">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C51">
-        <v>384</v>
+        <v>138</v>
       </c>
       <c r="D51">
         <v>124</v>
@@ -9990,10 +9972,10 @@
     </row>
     <row r="52" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
-        <v>249</v>
+        <v>139</v>
       </c>
       <c r="C52">
-        <v>383</v>
+        <v>88</v>
       </c>
       <c r="D52">
         <v>137</v>
@@ -10124,10 +10106,10 @@
     </row>
     <row r="53" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
-        <v>251</v>
+        <v>125</v>
       </c>
       <c r="C53">
-        <v>381</v>
+        <v>81</v>
       </c>
       <c r="D53">
         <v>137</v>
@@ -10243,7 +10225,10 @@
     </row>
     <row r="54" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
-        <v>250</v>
+        <v>140</v>
+      </c>
+      <c r="C54">
+        <v>83</v>
       </c>
       <c r="D54">
         <v>137</v>
@@ -10353,7 +10338,10 @@
     </row>
     <row r="55" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
-        <v>249</v>
+        <v>140</v>
+      </c>
+      <c r="C55">
+        <v>138</v>
       </c>
       <c r="D55">
         <v>137</v>
@@ -10460,7 +10448,10 @@
     </row>
     <row r="56" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
-        <v>252</v>
+        <v>133</v>
+      </c>
+      <c r="C56">
+        <v>84</v>
       </c>
       <c r="D56">
         <v>137</v>
@@ -10567,7 +10558,10 @@
     </row>
     <row r="57" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
-        <v>275</v>
+        <v>115</v>
+      </c>
+      <c r="C57">
+        <v>140</v>
       </c>
       <c r="D57">
         <v>137</v>
@@ -10671,7 +10665,10 @@
     </row>
     <row r="58" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
-        <v>249</v>
+        <v>139</v>
+      </c>
+      <c r="C58">
+        <v>140</v>
       </c>
       <c r="D58">
         <v>137</v>
@@ -10775,7 +10772,10 @@
     </row>
     <row r="59" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
-        <v>250</v>
+        <v>124</v>
+      </c>
+      <c r="C59">
+        <v>90</v>
       </c>
       <c r="D59">
         <v>137</v>
@@ -10876,7 +10876,10 @@
     </row>
     <row r="60" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
-        <v>250</v>
+        <v>1011</v>
+      </c>
+      <c r="C60">
+        <v>91</v>
       </c>
       <c r="D60">
         <v>137</v>
@@ -10974,7 +10977,7 @@
     </row>
     <row r="61" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
-        <v>251</v>
+        <v>137</v>
       </c>
       <c r="D61">
         <v>137</v>
@@ -11069,7 +11072,7 @@
     </row>
     <row r="62" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
-        <v>250</v>
+        <v>130</v>
       </c>
       <c r="D62">
         <v>137</v>
@@ -11158,7 +11161,7 @@
     </row>
     <row r="63" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
-        <v>249</v>
+        <v>138</v>
       </c>
       <c r="D63">
         <v>136</v>
@@ -11247,7 +11250,7 @@
     </row>
     <row r="64" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
-        <v>251</v>
+        <v>139</v>
       </c>
       <c r="D64">
         <v>137</v>
@@ -11330,7 +11333,7 @@
     </row>
     <row r="65" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
-        <v>251</v>
+        <v>144</v>
       </c>
       <c r="D65">
         <v>137</v>
@@ -11413,7 +11416,7 @@
     </row>
     <row r="66" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
-        <v>250</v>
+        <v>141</v>
       </c>
       <c r="D66">
         <v>137</v>
@@ -11493,7 +11496,7 @@
     </row>
     <row r="67" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
-        <v>250</v>
+        <v>138</v>
       </c>
       <c r="D67">
         <v>137</v>
@@ -11573,7 +11576,7 @@
     </row>
     <row r="68" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
-        <v>250</v>
+        <v>137</v>
       </c>
       <c r="D68">
         <v>137</v>
@@ -11647,7 +11650,7 @@
     </row>
     <row r="69" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
-        <v>252</v>
+        <v>140</v>
       </c>
       <c r="D69">
         <v>138</v>
@@ -11709,7 +11712,7 @@
     </row>
     <row r="70" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
-        <v>251</v>
+        <v>138</v>
       </c>
       <c r="D70">
         <v>137</v>
@@ -11771,7 +11774,7 @@
     </row>
     <row r="71" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
-        <v>251</v>
+        <v>138</v>
       </c>
       <c r="D71">
         <v>138</v>
@@ -11832,6 +11835,9 @@
       </c>
     </row>
     <row r="72" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72">
+        <v>140</v>
+      </c>
       <c r="D72">
         <v>137</v>
       </c>
@@ -11891,6 +11897,9 @@
       </c>
     </row>
     <row r="73" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73">
+        <v>148</v>
+      </c>
       <c r="D73">
         <v>137</v>
       </c>

</xml_diff>